<commit_message>
FIX: Modificación Clasificador Presupuestario.xlsx
</commit_message>
<xml_diff>
--- a/applications/formularios_sectoriales/Clasificador Presupuestario.xlsx
+++ b/applications/formularios_sectoriales/Clasificador Presupuestario.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaime\Desktop\SUBDERE\Transferencia de Competencias\transferenciacompetencias\applications\formularios_sectoriales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD1630B-D909-445D-B27C-7B6CB4B3ED07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EDA04F2-92CC-429E-B3BC-F5061798B78B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
   <si>
     <t>Sub. 21</t>
   </si>
@@ -296,7 +296,13 @@
     <t>012 - Otros Gastos en Bienes y Servicios de Consumo</t>
   </si>
   <si>
-    <t>Sin ítem</t>
+    <t>Sin ítem - Sub. 27</t>
+  </si>
+  <si>
+    <t>Sin ítem - Sub. 28</t>
+  </si>
+  <si>
+    <t>Sin ítem - Sub. 35</t>
   </si>
 </sst>
 </file>
@@ -622,18 +628,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" customWidth="1"/>
-    <col min="2" max="2" width="30.5703125" customWidth="1"/>
-    <col min="3" max="15" width="33.28515625" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" customWidth="1"/>
+    <col min="2" max="2" width="30.5546875" customWidth="1"/>
+    <col min="3" max="15" width="33.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -680,7 +686,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -703,7 +709,7 @@
         <v>86</v>
       </c>
       <c r="H2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I2" t="s">
         <v>21</v>
@@ -724,10 +730,10 @@
         <v>26</v>
       </c>
       <c r="O2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -765,7 +771,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -803,7 +809,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>51</v>
       </c>
@@ -835,7 +841,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>61</v>
       </c>
@@ -855,7 +861,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>67</v>
       </c>
@@ -875,7 +881,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>73</v>
       </c>
@@ -895,7 +901,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>79</v>
       </c>
@@ -906,22 +912,22 @@
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>85</v>
       </c>

</xml_diff>